<commit_message>
chap 10 vs grAss
</commit_message>
<xml_diff>
--- a/GroupAssginment.xlsx
+++ b/GroupAssginment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="12300"/>
+    <workbookView windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF434343"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. </t>
     </r>
     <r>
@@ -44,30 +51,55 @@
     </r>
   </si>
   <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRomanPS-BoldMT"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> Inventory turnover</t>
+    </r>
+  </si>
+  <si>
     <t>VINACHEM</t>
   </si>
   <si>
     <t>Net Sales</t>
   </si>
   <si>
+    <t>COGS</t>
+  </si>
+  <si>
     <t>Average Account Receivable</t>
   </si>
   <si>
+    <t>Average Inventory</t>
+  </si>
+  <si>
     <t>Account Receivable Tunover</t>
+  </si>
+  <si>
+    <t>Inventory Tunover</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +115,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF434343"/>
+      <name val="TimesNewRomanPS-BoldMT"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -225,6 +264,13 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="TimesNewRomanPS-BoldMT"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -554,137 +600,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -697,7 +743,16 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1233,13 +1288,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="8.01904761904762" customWidth="1"/>
     <col min="4" max="4" width="25"/>
@@ -1247,14 +1302,17 @@
     <col min="6" max="6" width="23.8571428571429"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.25" spans="1:1">
+    <row r="1" ht="23.25" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="I1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>2021</v>
@@ -1265,46 +1323,209 @@
       <c r="F4">
         <v>2023</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="I4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>2021</v>
+      </c>
+      <c r="M4">
+        <v>2022</v>
+      </c>
+      <c r="N4">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>47890935603429</v>
+      </c>
       <c r="E5" s="3">
         <v>56493459719089</v>
       </c>
       <c r="F5" s="3">
         <v>50572112579125</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <f>(3370146016319+4058358255565)/2</f>
+        <v>3714252135942</v>
+      </c>
+      <c r="E6" s="3">
+        <f>(4479112127897+3370146016319)/2</f>
+        <v>3924629072108</v>
+      </c>
       <c r="F6" s="3">
         <f>(4487713434899+4337363388244)/2</f>
         <v>4412538411571.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4">
+        <f>D5/D6</f>
+        <v>12.8938299960843</v>
+      </c>
+      <c r="E7" s="5">
+        <f>E5/E6</f>
+        <v>14.3945984909971</v>
+      </c>
+      <c r="F7" s="5">
         <f>F5/F6</f>
         <v>11.461002230939</v>
       </c>
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="10" spans="4:6">
+      <c r="D10">
+        <v>2021</v>
+      </c>
+      <c r="E10">
+        <v>2022</v>
+      </c>
+      <c r="F10">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="16" spans="4:6">
+      <c r="D16">
+        <v>2021</v>
+      </c>
+      <c r="E16">
+        <v>2022</v>
+      </c>
+      <c r="F16">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="22" spans="4:6">
+      <c r="D22">
+        <v>2021</v>
+      </c>
+      <c r="E22">
+        <v>2022</v>
+      </c>
+      <c r="F22">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="20">
     <mergeCell ref="A4:C4"/>
+    <mergeCell ref="I4:K4"/>
     <mergeCell ref="A5:C5"/>
+    <mergeCell ref="I5:K5"/>
     <mergeCell ref="A6:C6"/>
+    <mergeCell ref="I6:K6"/>
     <mergeCell ref="A7:C7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>